<commit_message>
Update base variables to source variables map
Make sure that every base variable present in the national data transformations are present in this spreadsheet
</commit_message>
<xml_diff>
--- a/analysis/data/ada_parc_base_variables_mapped_to_source_variables.xlsx
+++ b/analysis/data/ada_parc_base_variables_mapped_to_source_variables.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janehuber/Developer/ADA-PARC/ADAPARCDataPipeline/analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A398C71-47A5-2948-8B79-2BEF0AAA9C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE2FB6D-A8A1-944F-9F1A-16FCD61DA13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="3960" windowWidth="24640" windowHeight="13900" xr2:uid="{EBFDD4DC-FF19-304F-B78B-57CF7AA8244F}"/>
+    <workbookView xWindow="25600" yWindow="-10800" windowWidth="15180" windowHeight="28800" xr2:uid="{EBFDD4DC-FF19-304F-B78B-57CF7AA8244F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$133</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="267">
   <si>
     <t>ada_parc_var_code</t>
   </si>
@@ -443,18 +443,12 @@
     <t>pwd_white_nonhisp</t>
   </si>
   <si>
-    <t>pop_18_64</t>
-  </si>
-  <si>
     <t>pwd_0_5</t>
   </si>
   <si>
     <t>pwd_5_17</t>
   </si>
   <si>
-    <t>pwd_18_64</t>
-  </si>
-  <si>
     <t>pop_grtoeq_65</t>
   </si>
   <si>
@@ -719,18 +713,12 @@
     <t>pwd_other_americanindian_alaskanative</t>
   </si>
   <si>
-    <t>pwd_other_asian</t>
-  </si>
-  <si>
     <t>pwd_other_nativehawaiian_otherpacificislander</t>
   </si>
   <si>
     <t>pwd_other_other_race</t>
   </si>
   <si>
-    <t>pwd_other_twoormoreraces</t>
-  </si>
-  <si>
     <t>pop_18_64_ages18to34</t>
   </si>
   <si>
@@ -749,13 +737,109 @@
     <t>pwd_grtoeq_65_75yrsplus</t>
   </si>
   <si>
-    <t>pop_total_civiliannoninstitutionalized</t>
-  </si>
-  <si>
     <t>pwd_18_64_noninstitutionalized18to34yrs</t>
   </si>
   <si>
     <t>pwd_18_64_noninstitutionalized35to64</t>
+  </si>
+  <si>
+    <t>pop_total_grpquarters</t>
+  </si>
+  <si>
+    <t>pwd_multiple</t>
+  </si>
+  <si>
+    <t>pwd_asian</t>
+  </si>
+  <si>
+    <t>pop_grpqrters_18_64</t>
+  </si>
+  <si>
+    <t>pwd_grpqrters_18_64</t>
+  </si>
+  <si>
+    <t>S2602_C04_047</t>
+  </si>
+  <si>
+    <t>S2602_C04_048</t>
+  </si>
+  <si>
+    <t>pop_nursing_18_64</t>
+  </si>
+  <si>
+    <t>S2602_C01_049</t>
+  </si>
+  <si>
+    <t>pwod_nursing_18_64_pct</t>
+  </si>
+  <si>
+    <t>pwd_nursing_18_64_pct</t>
+  </si>
+  <si>
+    <t>pwd_corrections_base_number</t>
+  </si>
+  <si>
+    <t>pwod_corrections_base_number</t>
+  </si>
+  <si>
+    <t>B26108_003</t>
+  </si>
+  <si>
+    <t>B26108_002</t>
+  </si>
+  <si>
+    <t>pop_total_commute</t>
+  </si>
+  <si>
+    <t>S1811_C01_032</t>
+  </si>
+  <si>
+    <t>pwd_pop_educ</t>
+  </si>
+  <si>
+    <t>S1811_C02_039</t>
+  </si>
+  <si>
+    <t>C18130_009</t>
+  </si>
+  <si>
+    <t>C18130_010</t>
+  </si>
+  <si>
+    <t>pwd_class_18_64</t>
+  </si>
+  <si>
+    <t>pop_total_class_18_64</t>
+  </si>
+  <si>
+    <t>pwod_class_18_64</t>
+  </si>
+  <si>
+    <t>C18130_013</t>
+  </si>
+  <si>
+    <t>B25091_002</t>
+  </si>
+  <si>
+    <t>total_housing_units_mortgage</t>
+  </si>
+  <si>
+    <t>B25070_001</t>
+  </si>
+  <si>
+    <t>rent_total</t>
+  </si>
+  <si>
+    <t>pwd_total_commute</t>
+  </si>
+  <si>
+    <t>S1811_C02_032</t>
+  </si>
+  <si>
+    <t>S1811_C03_032</t>
+  </si>
+  <si>
+    <t>pwod_total_commute</t>
   </si>
 </sst>
 </file>
@@ -797,7 +881,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1107,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11ECB4C-D257-3344-82DA-938265661733}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,13 +1230,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D2">
         <v>2021</v>
@@ -1155,7 +1250,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D3">
         <v>2021</v>
@@ -1169,7 +1264,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D4">
         <v>2021</v>
@@ -1183,7 +1278,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D5">
         <v>2021</v>
@@ -1197,7 +1292,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D6">
         <v>2021</v>
@@ -1211,7 +1306,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D7">
         <v>2021</v>
@@ -1225,7 +1320,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D8">
         <v>2021</v>
@@ -1239,7 +1334,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D9">
         <v>2021</v>
@@ -1253,7 +1348,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D10">
         <v>2021</v>
@@ -1267,7 +1362,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D11">
         <v>2021</v>
@@ -1281,7 +1376,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D12">
         <v>2021</v>
@@ -1295,7 +1390,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D13">
         <v>2021</v>
@@ -1303,13 +1398,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D14">
         <v>2021</v>
@@ -1317,13 +1412,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D15">
         <v>2021</v>
@@ -1331,13 +1426,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D16">
         <v>2021</v>
@@ -1345,13 +1440,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D17">
         <v>2021</v>
@@ -1359,13 +1454,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D18">
         <v>2021</v>
@@ -1373,13 +1468,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D19">
         <v>2021</v>
@@ -1387,13 +1482,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D20">
         <v>2021</v>
@@ -1401,13 +1496,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D21">
         <v>2021</v>
@@ -1415,13 +1510,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D22">
         <v>2021</v>
@@ -1429,13 +1524,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D23">
         <v>2021</v>
@@ -1443,13 +1538,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D24">
         <v>2021</v>
@@ -1457,13 +1552,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D25">
         <v>2021</v>
@@ -1471,13 +1566,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D26">
         <v>2021</v>
@@ -1485,13 +1580,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D27">
         <v>2021</v>
@@ -1499,13 +1594,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D28">
         <v>2021</v>
@@ -1513,13 +1608,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D29">
         <v>2021</v>
@@ -1527,13 +1622,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D30">
         <v>2021</v>
@@ -1541,13 +1636,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D31">
         <v>2021</v>
@@ -1555,13 +1650,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D32">
         <v>2021</v>
@@ -1569,13 +1664,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>234</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D33">
         <v>2021</v>
@@ -1589,7 +1684,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D34">
         <v>2021</v>
@@ -1597,13 +1692,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D35">
         <v>2021</v>
@@ -1611,13 +1706,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D36">
         <v>2021</v>
@@ -1625,13 +1720,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D37">
         <v>2021</v>
@@ -1639,13 +1734,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D38">
         <v>2021</v>
@@ -1653,13 +1748,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D39">
         <v>2021</v>
@@ -1667,13 +1762,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D40">
         <v>2021</v>
@@ -1681,13 +1776,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B41" t="s">
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D41">
         <v>2021</v>
@@ -1695,13 +1790,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>237</v>
       </c>
       <c r="B42" t="s">
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D42">
         <v>2021</v>
@@ -1709,13 +1804,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>238</v>
       </c>
       <c r="B43" t="s">
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D43">
         <v>2021</v>
@@ -1723,13 +1818,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>241</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>239</v>
       </c>
       <c r="C44" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D44">
         <v>2021</v>
@@ -1737,13 +1832,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>244</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>240</v>
       </c>
       <c r="C45" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D45">
         <v>2021</v>
@@ -1751,13 +1846,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>242</v>
       </c>
       <c r="C46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D46">
         <v>2021</v>
@@ -1765,13 +1860,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D47">
         <v>2021</v>
@@ -1779,13 +1874,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D48">
         <v>2021</v>
@@ -1793,13 +1888,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D49">
         <v>2021</v>
@@ -1807,13 +1902,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D50">
         <v>2021</v>
@@ -1821,13 +1916,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D51">
         <v>2021</v>
@@ -1835,13 +1930,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D52">
         <v>2021</v>
@@ -1849,13 +1944,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D53">
         <v>2021</v>
@@ -1863,13 +1958,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>138</v>
+        <v>245</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>248</v>
       </c>
       <c r="C54" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D54">
         <v>2021</v>
@@ -1877,13 +1972,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>139</v>
+        <v>246</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>247</v>
       </c>
       <c r="C55" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D55">
         <v>2021</v>
@@ -1891,13 +1986,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D56">
         <v>2021</v>
@@ -1905,13 +2000,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D57">
         <v>2021</v>
@@ -1919,13 +2014,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D58">
         <v>2021</v>
@@ -1933,13 +2028,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D59">
         <v>2021</v>
@@ -1947,13 +2042,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D60">
         <v>2021</v>
@@ -1961,13 +2056,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C61" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D61">
         <v>2021</v>
@@ -1975,13 +2070,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C62" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D62">
         <v>2021</v>
@@ -1989,13 +2084,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C63" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D63">
         <v>2021</v>
@@ -2003,13 +2098,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D64">
         <v>2021</v>
@@ -2017,13 +2112,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D65">
         <v>2021</v>
@@ -2031,13 +2126,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C66" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D66">
         <v>2021</v>
@@ -2045,13 +2140,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D67">
         <v>2021</v>
@@ -2059,13 +2154,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D68">
         <v>2021</v>
@@ -2073,13 +2168,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D69">
         <v>2021</v>
@@ -2087,13 +2182,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D70">
         <v>2021</v>
@@ -2101,13 +2196,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D71">
         <v>2021</v>
@@ -2115,13 +2210,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D72">
         <v>2021</v>
@@ -2129,13 +2224,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D73">
         <v>2021</v>
@@ -2143,13 +2238,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D74">
         <v>2021</v>
@@ -2157,13 +2252,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C75" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D75">
         <v>2021</v>
@@ -2171,13 +2266,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D76">
         <v>2021</v>
@@ -2185,13 +2280,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D77">
         <v>2021</v>
@@ -2199,13 +2294,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>183</v>
+        <v>249</v>
       </c>
       <c r="B78" t="s">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="C78" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D78">
         <v>2021</v>
@@ -2213,13 +2308,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>184</v>
+        <v>263</v>
       </c>
       <c r="B79" t="s">
-        <v>81</v>
+        <v>264</v>
       </c>
       <c r="C79" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D79">
         <v>2021</v>
@@ -2227,13 +2322,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>185</v>
+        <v>266</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>265</v>
       </c>
       <c r="C80" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D80">
         <v>2021</v>
@@ -2241,13 +2336,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C81" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D81">
         <v>2021</v>
@@ -2255,13 +2350,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C82" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D82">
         <v>2021</v>
@@ -2269,13 +2364,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C83" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D83">
         <v>2021</v>
@@ -2283,13 +2378,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C84" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D84">
         <v>2021</v>
@@ -2297,13 +2392,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C85" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D85">
         <v>2021</v>
@@ -2311,13 +2406,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C86" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D86">
         <v>2021</v>
@@ -2325,13 +2420,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>192</v>
+        <v>251</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
+        <v>252</v>
       </c>
       <c r="C87" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D87">
         <v>2021</v>
@@ -2339,13 +2434,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D88">
         <v>2021</v>
@@ -2353,13 +2448,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B89" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C89" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D89">
         <v>2021</v>
@@ -2367,13 +2462,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C90" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D90">
         <v>2021</v>
@@ -2381,13 +2476,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B91" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C91" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D91">
         <v>2021</v>
@@ -2395,13 +2490,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B92" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C92" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D92">
         <v>2021</v>
@@ -2409,13 +2504,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C93" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D93">
         <v>2021</v>
@@ -2423,13 +2518,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B94" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C94" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D94">
         <v>2021</v>
@@ -2437,13 +2532,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B95" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C95" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D95">
         <v>2021</v>
@@ -2451,13 +2546,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>201</v>
+        <v>256</v>
       </c>
       <c r="B96" t="s">
-        <v>98</v>
+        <v>253</v>
       </c>
       <c r="C96" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D96">
         <v>2021</v>
@@ -2465,13 +2560,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
+        <v>254</v>
       </c>
       <c r="C97" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D97">
         <v>2021</v>
@@ -2479,13 +2574,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>203</v>
+        <v>257</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
+        <v>258</v>
       </c>
       <c r="C98" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D98">
         <v>2021</v>
@@ -2493,13 +2588,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B99" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C99" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D99">
         <v>2021</v>
@@ -2507,13 +2602,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B100" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C100" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D100">
         <v>2021</v>
@@ -2521,13 +2616,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C101" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D101">
         <v>2021</v>
@@ -2535,13 +2630,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="B102" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C102" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D102">
         <v>2021</v>
@@ -2549,13 +2644,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B103" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C103" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D103">
         <v>2021</v>
@@ -2563,13 +2658,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B104" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C104" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D104">
         <v>2021</v>
@@ -2577,13 +2672,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B105" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C105" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D105">
         <v>2021</v>
@@ -2591,13 +2686,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B106" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C106" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D106">
         <v>2021</v>
@@ -2605,13 +2700,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B107" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C107" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D107">
         <v>2021</v>
@@ -2619,13 +2714,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B108" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C108" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D108">
         <v>2021</v>
@@ -2633,13 +2728,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C109" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D109">
         <v>2021</v>
@@ -2647,13 +2742,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B110" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C110" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D110">
         <v>2021</v>
@@ -2661,13 +2756,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="B111" t="s">
-        <v>113</v>
+        <v>259</v>
       </c>
       <c r="C111" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D111">
         <v>2021</v>
@@ -2675,13 +2770,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B112" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C112" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D112">
         <v>2021</v>
@@ -2689,13 +2784,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C113" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D113">
         <v>2021</v>
@@ -2703,13 +2798,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="B114" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C114" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D114">
         <v>2021</v>
@@ -2717,13 +2812,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B115" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C115" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D115">
         <v>2021</v>
@@ -2731,13 +2826,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>221</v>
+        <v>262</v>
       </c>
       <c r="B116" t="s">
-        <v>118</v>
+        <v>261</v>
       </c>
       <c r="C116" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D116">
         <v>2021</v>
@@ -2745,13 +2840,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B117" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C117" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D117">
         <v>2021</v>
@@ -2759,20 +2854,219 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B118" t="s">
+        <v>106</v>
+      </c>
+      <c r="C118" t="s">
+        <v>222</v>
+      </c>
+      <c r="D118">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>208</v>
+      </c>
+      <c r="B119" t="s">
+        <v>107</v>
+      </c>
+      <c r="C119" t="s">
+        <v>222</v>
+      </c>
+      <c r="D119">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>209</v>
+      </c>
+      <c r="B120" t="s">
+        <v>108</v>
+      </c>
+      <c r="C120" t="s">
+        <v>222</v>
+      </c>
+      <c r="D120">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>210</v>
+      </c>
+      <c r="B121" t="s">
+        <v>109</v>
+      </c>
+      <c r="C121" t="s">
+        <v>222</v>
+      </c>
+      <c r="D121">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>211</v>
+      </c>
+      <c r="B122" t="s">
+        <v>110</v>
+      </c>
+      <c r="C122" t="s">
+        <v>222</v>
+      </c>
+      <c r="D122">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>212</v>
+      </c>
+      <c r="B123" t="s">
+        <v>111</v>
+      </c>
+      <c r="C123" t="s">
+        <v>222</v>
+      </c>
+      <c r="D123">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>213</v>
+      </c>
+      <c r="B124" t="s">
+        <v>112</v>
+      </c>
+      <c r="C124" t="s">
+        <v>222</v>
+      </c>
+      <c r="D124">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>214</v>
+      </c>
+      <c r="B125" t="s">
+        <v>113</v>
+      </c>
+      <c r="C125" t="s">
+        <v>222</v>
+      </c>
+      <c r="D125">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>215</v>
+      </c>
+      <c r="B126" t="s">
+        <v>114</v>
+      </c>
+      <c r="C126" t="s">
+        <v>222</v>
+      </c>
+      <c r="D126">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>216</v>
+      </c>
+      <c r="B127" t="s">
+        <v>115</v>
+      </c>
+      <c r="C127" t="s">
+        <v>222</v>
+      </c>
+      <c r="D127">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>217</v>
+      </c>
+      <c r="B128" t="s">
+        <v>116</v>
+      </c>
+      <c r="C128" t="s">
+        <v>222</v>
+      </c>
+      <c r="D128">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>218</v>
+      </c>
+      <c r="B129" t="s">
+        <v>117</v>
+      </c>
+      <c r="C129" t="s">
+        <v>222</v>
+      </c>
+      <c r="D129">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>219</v>
+      </c>
+      <c r="B130" t="s">
+        <v>118</v>
+      </c>
+      <c r="C130" t="s">
+        <v>222</v>
+      </c>
+      <c r="D130">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>220</v>
+      </c>
+      <c r="B131" t="s">
+        <v>119</v>
+      </c>
+      <c r="C131" t="s">
+        <v>222</v>
+      </c>
+      <c r="D131">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>221</v>
+      </c>
+      <c r="B132" t="s">
         <v>120</v>
       </c>
-      <c r="C118" t="s">
-        <v>224</v>
-      </c>
-      <c r="D118">
+      <c r="C132" t="s">
+        <v>222</v>
+      </c>
+      <c r="D132">
         <v>2021</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A118" xr:uid="{A11ECB4C-D257-3344-82DA-938265661733}"/>
+  <autoFilter ref="B1:B133" xr:uid="{A11ECB4C-D257-3344-82DA-938265661733}"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update vars in calculations for participation
</commit_message>
<xml_diff>
--- a/analysis/data/ada_parc_base_variables_mapped_to_source_variables.xlsx
+++ b/analysis/data/ada_parc_base_variables_mapped_to_source_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janehuber/Developer/ADA-PARC/ADAPARCDataPipeline/analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1B8966-EFBA-5D4A-BA03-8918595B87B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A699BD2-46C8-A34E-83E0-987B1E558015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="5" xr2:uid="{EBFDD4DC-FF19-304F-B78B-57CF7AA8244F}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="2016" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2021'!$B$1:$B$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2021'!$B$1:$B$135</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2385" uniqueCount="273">
   <si>
     <t>ada_parc_var_code</t>
   </si>
@@ -857,13 +857,19 @@
   </si>
   <si>
     <t>B26108_039</t>
+  </si>
+  <si>
+    <t>S1811_C03_039</t>
+  </si>
+  <si>
+    <t>pwod_pop_educ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -877,6 +883,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -899,9 +911,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1307,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11ECB4C-D257-3344-82DA-938265661733}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2553,10 +2566,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
       <c r="B89" t="s">
-        <v>250</v>
+        <v>271</v>
       </c>
       <c r="C89" t="s">
         <v>222</v>
@@ -2567,10 +2580,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>182</v>
+        <v>249</v>
       </c>
       <c r="B90" t="s">
-        <v>81</v>
+        <v>250</v>
       </c>
       <c r="C90" t="s">
         <v>222</v>
@@ -2581,10 +2594,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B91" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C91" t="s">
         <v>222</v>
@@ -2595,10 +2608,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B92" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C92" t="s">
         <v>222</v>
@@ -2609,10 +2622,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B93" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C93" t="s">
         <v>222</v>
@@ -2623,10 +2636,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B94" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C94" t="s">
         <v>222</v>
@@ -2637,10 +2650,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B95" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C95" t="s">
         <v>222</v>
@@ -2651,10 +2664,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B96" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C96" t="s">
         <v>222</v>
@@ -2665,10 +2678,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B97" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C97" t="s">
         <v>222</v>
@@ -2679,10 +2692,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>254</v>
+        <v>189</v>
       </c>
       <c r="B98" t="s">
-        <v>251</v>
+        <v>88</v>
       </c>
       <c r="C98" t="s">
         <v>222</v>
@@ -2693,10 +2706,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C99" t="s">
         <v>222</v>
@@ -2707,10 +2720,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B100" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C100" t="s">
         <v>222</v>
@@ -2721,10 +2734,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>190</v>
+        <v>255</v>
       </c>
       <c r="B101" t="s">
-        <v>89</v>
+        <v>256</v>
       </c>
       <c r="C101" t="s">
         <v>222</v>
@@ -2735,10 +2748,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C102" t="s">
         <v>222</v>
@@ -2749,10 +2762,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C103" t="s">
         <v>222</v>
@@ -2763,10 +2776,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C104" t="s">
         <v>222</v>
@@ -2777,10 +2790,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B105" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C105" t="s">
         <v>222</v>
@@ -2791,10 +2804,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B106" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C106" t="s">
         <v>222</v>
@@ -2805,10 +2818,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B107" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C107" t="s">
         <v>222</v>
@@ -2819,10 +2832,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B108" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C108" t="s">
         <v>222</v>
@@ -2833,10 +2846,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B109" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C109" t="s">
         <v>222</v>
@@ -2847,10 +2860,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B110" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C110" t="s">
         <v>222</v>
@@ -2861,10 +2874,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B111" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C111" t="s">
         <v>222</v>
@@ -2875,10 +2888,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B112" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C112" t="s">
         <v>222</v>
@@ -2889,10 +2902,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>258</v>
+        <v>201</v>
       </c>
       <c r="B113" t="s">
-        <v>257</v>
+        <v>100</v>
       </c>
       <c r="C113" t="s">
         <v>222</v>
@@ -2903,10 +2916,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>202</v>
+        <v>258</v>
       </c>
       <c r="B114" t="s">
-        <v>101</v>
+        <v>257</v>
       </c>
       <c r="C114" t="s">
         <v>222</v>
@@ -2917,10 +2930,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B115" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C115" t="s">
         <v>222</v>
@@ -2931,10 +2944,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B116" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C116" t="s">
         <v>222</v>
@@ -2945,10 +2958,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B117" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C117" t="s">
         <v>222</v>
@@ -2959,10 +2972,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>260</v>
+        <v>205</v>
       </c>
       <c r="B118" t="s">
-        <v>259</v>
+        <v>104</v>
       </c>
       <c r="C118" t="s">
         <v>222</v>
@@ -2973,10 +2986,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>206</v>
+        <v>260</v>
       </c>
       <c r="B119" t="s">
-        <v>105</v>
+        <v>259</v>
       </c>
       <c r="C119" t="s">
         <v>222</v>
@@ -2987,10 +3000,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B120" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C120" t="s">
         <v>222</v>
@@ -3001,10 +3014,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B121" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C121" t="s">
         <v>222</v>
@@ -3015,10 +3028,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B122" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C122" t="s">
         <v>222</v>
@@ -3029,10 +3042,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B123" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C123" t="s">
         <v>222</v>
@@ -3043,10 +3056,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C124" t="s">
         <v>222</v>
@@ -3057,10 +3070,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C125" t="s">
         <v>222</v>
@@ -3071,10 +3084,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B126" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C126" t="s">
         <v>222</v>
@@ -3085,10 +3098,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B127" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C127" t="s">
         <v>222</v>
@@ -3099,10 +3112,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B128" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C128" t="s">
         <v>222</v>
@@ -3113,10 +3126,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B129" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C129" t="s">
         <v>222</v>
@@ -3127,10 +3140,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B130" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C130" t="s">
         <v>222</v>
@@ -3141,10 +3154,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B131" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C131" t="s">
         <v>222</v>
@@ -3155,10 +3168,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C132" t="s">
         <v>222</v>
@@ -3169,10 +3182,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B133" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C133" t="s">
         <v>222</v>
@@ -3183,21 +3196,38 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>220</v>
+      </c>
+      <c r="B134" t="s">
+        <v>119</v>
+      </c>
+      <c r="C134" t="s">
+        <v>222</v>
+      </c>
+      <c r="D134">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>221</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B135" t="s">
         <v>120</v>
       </c>
-      <c r="C134" t="s">
-        <v>222</v>
-      </c>
-      <c r="D134">
-        <v>2021</v>
-      </c>
+      <c r="C135" t="s">
+        <v>222</v>
+      </c>
+      <c r="D135">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B136" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B134" xr:uid="{A11ECB4C-D257-3344-82DA-938265661733}"/>
-  <conditionalFormatting sqref="B1:B1048576">
+  <autoFilter ref="B1:B135" xr:uid="{A11ECB4C-D257-3344-82DA-938265661733}"/>
+  <conditionalFormatting sqref="B137:B1048576 B1:B135">
     <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3206,10 +3236,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE569FCC-3177-F34C-A933-0E5C16F88663}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D135"/>
   <sheetViews>
     <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133:D134"/>
+      <selection activeCell="A135" sqref="A135:C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5094,8 +5124,25 @@
         <v>2020</v>
       </c>
     </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>272</v>
+      </c>
+      <c r="B135" t="s">
+        <v>271</v>
+      </c>
+      <c r="C135" t="s">
+        <v>222</v>
+      </c>
+      <c r="D135">
+        <v>2020</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:B134 B136:B1048576">
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B135">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5104,10 +5151,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BFE289-18F6-ED41-85D8-276C2D8F5175}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D135"/>
   <sheetViews>
     <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133:D134"/>
+      <selection activeCell="A135" sqref="A135:C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6992,8 +7039,25 @@
         <v>2019</v>
       </c>
     </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>272</v>
+      </c>
+      <c r="B135" t="s">
+        <v>271</v>
+      </c>
+      <c r="C135" t="s">
+        <v>222</v>
+      </c>
+      <c r="D135" s="1">
+        <v>2019</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:B134 B136:B1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B135">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7002,10 +7066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE2D87A-6C02-9E40-A903-7D79AC15372A}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D135"/>
   <sheetViews>
     <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133:D134"/>
+      <selection activeCell="A135" sqref="A135:C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8890,8 +8954,25 @@
         <v>2018</v>
       </c>
     </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>272</v>
+      </c>
+      <c r="B135" t="s">
+        <v>271</v>
+      </c>
+      <c r="C135" t="s">
+        <v>222</v>
+      </c>
+      <c r="D135" s="1">
+        <v>2018</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:B134 B136:B1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B135">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8900,10 +8981,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A03A2AE-F19F-2746-8652-3E8E28F1D4C8}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D135"/>
   <sheetViews>
     <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+      <selection activeCell="A135" sqref="A135:C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10788,8 +10869,25 @@
         <v>2017</v>
       </c>
     </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>272</v>
+      </c>
+      <c r="B135" t="s">
+        <v>271</v>
+      </c>
+      <c r="C135" t="s">
+        <v>222</v>
+      </c>
+      <c r="D135" s="1">
+        <v>2017</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:B134 B136:B1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B135">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10798,10 +10896,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FD4663-240D-D04A-898E-0C5EE9C73613}">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117:D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12448,6 +12546,20 @@
         <v>2016</v>
       </c>
     </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D118" s="1">
+        <v>2016</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Need unique name for the subject table employment vars
</commit_message>
<xml_diff>
--- a/analysis/data/ada_parc_base_variables_mapped_to_source_variables.xlsx
+++ b/analysis/data/ada_parc_base_variables_mapped_to_source_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janehuber/Developer/ADA-PARC/ADAPARCDataPipeline/analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3945CEE0-AB7A-B545-84BF-3B728E21AB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDB84F1-DA2A-C540-A23E-854ADEE003ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="5" xr2:uid="{EBFDD4DC-FF19-304F-B78B-57CF7AA8244F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="4" xr2:uid="{EBFDD4DC-FF19-304F-B78B-57CF7AA8244F}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2508" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2508" uniqueCount="289">
   <si>
     <t>ada_parc_var_code</t>
   </si>
@@ -901,13 +901,16 @@
     <t>S1811_C02_001</t>
   </si>
   <si>
-    <t>pwd_16_plus</t>
-  </si>
-  <si>
     <t>S1811_C02_003</t>
   </si>
   <si>
-    <t>pwd_not_employed</t>
+    <t>pwd_not_employed_subj</t>
+  </si>
+  <si>
+    <t>pwd_employed_subj</t>
+  </si>
+  <si>
+    <t>pwd_16_plus_subj</t>
   </si>
 </sst>
 </file>
@@ -960,7 +963,97 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1403,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11ECB4C-D257-3344-82DA-938265661733}">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144:XFD144"/>
+    <sheetView topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141:B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3375,7 +3468,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>194</v>
+        <v>287</v>
       </c>
       <c r="B141" t="s">
         <v>282</v>
@@ -3389,7 +3482,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B142" t="s">
         <v>284</v>
@@ -3403,10 +3496,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B143" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C143" t="s">
         <v>222</v>
@@ -3418,7 +3511,7 @@
   </sheetData>
   <autoFilter ref="B1:B135" xr:uid="{A11ECB4C-D257-3344-82DA-938265661733}"/>
   <conditionalFormatting sqref="B1:B143 B145:B1048576">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3428,8 +3521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE569FCC-3177-F34C-A933-0E5C16F88663}">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144:XFD144"/>
+    <sheetView topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141:B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5400,7 +5493,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>194</v>
+        <v>287</v>
       </c>
       <c r="B141" t="s">
         <v>282</v>
@@ -5414,7 +5507,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B142" t="s">
         <v>284</v>
@@ -5428,10 +5521,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B143" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C143" t="s">
         <v>222</v>
@@ -5442,13 +5535,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B134 B145:B1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B135">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B136:B143">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+  <conditionalFormatting sqref="B136:B140">
+    <cfRule type="duplicateValues" dxfId="18" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B141:B143">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5458,8 +5554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BFE289-18F6-ED41-85D8-276C2D8F5175}">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144:XFD144"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141:B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7430,7 +7526,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>194</v>
+        <v>287</v>
       </c>
       <c r="B141" t="s">
         <v>282</v>
@@ -7444,7 +7540,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B142" t="s">
         <v>284</v>
@@ -7458,10 +7554,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B143" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C143" t="s">
         <v>222</v>
@@ -7472,13 +7568,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B134 B145:B1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B135">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B136:B143">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+  <conditionalFormatting sqref="B136:B140">
+    <cfRule type="duplicateValues" dxfId="15" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B141:B143">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7489,7 +7588,7 @@
   <dimension ref="A1:D144"/>
   <sheetViews>
     <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144:XFD144"/>
+      <selection activeCell="A141" sqref="A141:B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9460,7 +9559,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>194</v>
+        <v>287</v>
       </c>
       <c r="B141" t="s">
         <v>282</v>
@@ -9474,7 +9573,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B142" t="s">
         <v>284</v>
@@ -9488,10 +9587,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B143" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C143" t="s">
         <v>222</v>
@@ -9508,13 +9607,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B134 B145:B1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B135">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B136:B143">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  <conditionalFormatting sqref="B136:B140">
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B141:B143">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9524,8 +9626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A03A2AE-F19F-2746-8652-3E8E28F1D4C8}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144:XFD144"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11496,7 +11598,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>194</v>
+        <v>287</v>
       </c>
       <c r="B141" t="s">
         <v>282</v>
@@ -11510,7 +11612,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B142" t="s">
         <v>284</v>
@@ -11524,10 +11626,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B143" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C143" t="s">
         <v>222</v>
@@ -11544,12 +11646,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B134 B145:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B135">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B136:B143">
+  <conditionalFormatting sqref="B136:B140">
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B141:B143">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11560,8 +11665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FD4663-240D-D04A-898E-0C5EE9C73613}">
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>